<commit_message>
Added LULU, ON, PANW models
</commit_message>
<xml_diff>
--- a/Growth Stocks/SNOW-fs-01112023-lmyol.xlsx
+++ b/Growth Stocks/SNOW-fs-01112023-lmyol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/growth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Growth Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228076E9-383E-784E-A2AD-0EA59880F4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3726ADC5-9008-CB41-9E5D-D5A4B4389B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
     <t>link</t>
   </si>
   <si>
-    <t>SNOW</t>
+    <t>Snowflake</t>
   </si>
 </sst>
 </file>
@@ -774,11 +774,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>